<commit_message>
NVIDIA FY2026 Q4 決算更新 + update-earnings ワークフロー新設
- workflows/update-earnings.md を新規作成（既存企業の決算更新手順）
- NVIDIA FY2026 Q4 の決算資料DL・データ抽出・xlsx生成・ページ生成を実行
- generate-data-json.js: 既存四半期ページが消えないよう hasPage 判定を修正
- generate-ir-links.js: FY2026 Q4 の IR資料リンクを追加
- analysis-text.json: 決算サマリーをカテゴリ別ブロックに分割（見やすさ改善）
- analyze-and-visualize.md: 定性情報のカテゴリ分割構成を明記

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/companies/nvidia/data/Financials.xlsx
+++ b/companies/nvidia/data/Financials.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
   <si>
     <t>期間</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>Q4</t>
-  </si>
-  <si>
-    <t>Q4予想</t>
   </si>
   <si>
     <t>売上高</t>
@@ -766,12 +763,12 @@
         <v>3</v>
       </c>
       <c r="Y2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="B3" s="4">
         <v>3080</v>
@@ -841,11 +838,14 @@
       </c>
       <c r="X3">
         <v>57006</v>
+      </c>
+      <c r="Y3">
+        <v>68127</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6">
@@ -920,7 +920,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -987,9 +987,9 @@
         <f>U3/Y3</f>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="10">
         <v>2004</v>
@@ -1060,10 +1060,13 @@
       <c r="X6">
         <v>41849</v>
       </c>
+      <c r="Y6">
+        <v>51093</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="12">
         <f>B6/B$3</f>
@@ -1133,11 +1136,14 @@
       </c>
       <c r="X7">
         <f>X6/X$3</f>
+      </c>
+      <c r="Y7">
+        <f>Y6/Y$3</f>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -1204,9 +1210,9 @@
         <f>Y6/U6</f>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="16">
         <v>735</v>
@@ -1276,11 +1282,14 @@
       </c>
       <c r="X9">
         <v>4705</v>
+      </c>
+      <c r="Y9">
+        <v>5512</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="18">
         <f>B9/B$3</f>
@@ -1355,9 +1364,9 @@
         <f>Y9/Y$3</f>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="16">
         <v>293</v>
@@ -1427,11 +1436,14 @@
       </c>
       <c r="X11">
         <v>1134</v>
+      </c>
+      <c r="Y11">
+        <v>1282</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="18">
         <f>B11/B$3</f>
@@ -1506,9 +1518,9 @@
         <f>Y11/Y$3</f>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="20">
         <v>1028</v>
@@ -1578,11 +1590,14 @@
       </c>
       <c r="X13">
         <v>5839</v>
+      </c>
+      <c r="Y13">
+        <v>6794</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="22">
         <f>B13/B$3</f>
@@ -1659,7 +1674,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
@@ -1726,9 +1741,9 @@
         <f>Y13/U13</f>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="10">
         <v>976</v>
@@ -1798,11 +1813,14 @@
       </c>
       <c r="X16">
         <v>36010</v>
+      </c>
+      <c r="Y16">
+        <v>44299</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="12">
         <f>B16/B$3</f>
@@ -1879,7 +1897,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -1946,9 +1964,9 @@
         <f>Y16/U16-1</f>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="24">
         <v>5</v>
@@ -2019,10 +2037,13 @@
       <c r="X19">
         <v>1926</v>
       </c>
+      <c r="Y19">
+        <v>6098</v>
+      </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="10">
         <v>917</v>
@@ -2093,10 +2114,13 @@
       <c r="X20">
         <v>31910</v>
       </c>
+      <c r="Y20">
+        <v>42960</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" s="12">
         <f>B20/B$3</f>
@@ -2166,11 +2190,14 @@
       </c>
       <c r="X21">
         <f>X20/X$3</f>
+      </c>
+      <c r="Y21">
+        <f>Y20/Y$3</f>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -2237,9 +2264,9 @@
         <f>Y20/U20-1</f>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="26">
         <v>0.04</v>
@@ -2309,11 +2336,14 @@
       </c>
       <c r="X23">
         <v>1.3</v>
+      </c>
+      <c r="Y23">
+        <v>1.76</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" s="28"/>
       <c r="C24" s="28"/>
@@ -2384,7 +2414,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="30"/>
       <c r="C25" s="30"/>
@@ -2447,9 +2477,9 @@
         <f>AVERAGE(V24:Y24)</f>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="31">
         <v>7.28</v>
@@ -2519,6 +2549,9 @@
       </c>
       <c r="X26">
         <v>201.03</v>
+      </c>
+      <c r="Y26">
+        <v>191.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>